<commit_message>
Add template for SWiM guidelines
</commit_message>
<xml_diff>
--- a/supplementary-material/inputs/prisma_checklist.xlsx
+++ b/supplementary-material/inputs/prisma_checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtay0016/dev/youth-homelessness-review/supplementary-material/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CF34CD-61AF-B148-9D7C-1F0F1532BE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03EE538C-32F6-BE40-9F02-E1851FAD01D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" xr2:uid="{A1839663-239A-1A4B-89C5-AE8F063D74BB}"/>
   </bookViews>
@@ -762,6 +762,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -778,9 +781,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1102,8 +1102,8 @@
   </sheetPr>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1127,11 +1127,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1149,11 +1149,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1171,11 +1171,11 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
@@ -1207,11 +1207,11 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" ht="40" thickBot="1" x14ac:dyDescent="0.25">
@@ -1224,7 +1224,7 @@
       <c r="C10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="20" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1252,7 +1252,7 @@
       <c r="C12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="20" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1378,7 +1378,7 @@
       <c r="C21" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="20" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1453,11 +1453,11 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="23"/>
       <c r="D27" s="19"/>
     </row>
     <row r="28" spans="1:4" ht="53" thickBot="1" x14ac:dyDescent="0.25">
@@ -1526,7 +1526,7 @@
       <c r="C32" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="26" t="s">
+      <c r="D32" s="20" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1615,11 +1615,11 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="20" t="s">
+      <c r="A39" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="22"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="23"/>
       <c r="D39" s="19"/>
     </row>
     <row r="40" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
@@ -1665,11 +1665,11 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="24"/>
-      <c r="C43" s="25"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="26"/>
       <c r="D43" s="19"/>
     </row>
     <row r="44" spans="1:4" ht="40" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>